<commit_message>
gantt + grill d'eval + maj diapo
</commit_message>
<xml_diff>
--- a/GANTT.xlsx
+++ b/GANTT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean Leduc\Desktop\Rapport-de-stage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanl\Desktop\Scolaire\BTS SN2\Rapport de stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CBF843-A749-48EA-9D7C-A8B96C559B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -26,8 +27,17 @@
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,57 +46,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -191,27 +153,9 @@
     <t>Plan Duration</t>
   </si>
   <si>
-    <t>PERIODS (h)</t>
-  </si>
-  <si>
-    <t>Classe</t>
-  </si>
-  <si>
-    <t>GANTT</t>
-  </si>
-  <si>
-    <t>Faire la bdd</t>
-  </si>
-  <si>
-    <t>Créer la page pour les administrateurs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Faire les affiches </t>
   </si>
   <si>
-    <t>Faire le deFaire l'analyse de référencement</t>
-  </si>
-  <si>
     <t>Faire le Benchmark</t>
   </si>
   <si>
@@ -225,12 +169,42 @@
   </si>
   <si>
     <t>Faire le site de réservation</t>
+  </si>
+  <si>
+    <t>Faire l'analyse de référencement</t>
+  </si>
+  <si>
+    <t>Page inscription/connexion</t>
+  </si>
+  <si>
+    <t>Page pour réserver</t>
+  </si>
+  <si>
+    <t>Créer la Base de Donnée</t>
+  </si>
+  <si>
+    <t>Page pour le menu des administrateurs</t>
+  </si>
+  <si>
+    <t>Accepter/refuser réservations</t>
+  </si>
+  <si>
+    <t>PERIODS (j)</t>
+  </si>
+  <si>
+    <t>Créer une réservation en administrateur</t>
+  </si>
+  <si>
+    <t>Voir visuellement les réservations</t>
+  </si>
+  <si>
+    <t>Pouvoir supprimer les réservations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,7 +320,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +365,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +518,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -593,17 +573,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
@@ -620,51 +606,54 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="10" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="10" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Texte explicatif" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Titre" xfId="8" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Titre 1" xfId="1" builtinId="16" customBuiltin="1"/>
@@ -1054,30 +1043,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:CS30"/>
+  <dimension ref="A1:CS18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="4.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="27" width="2.75" style="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="2" customWidth="1"/>
+    <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="27" width="2.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:97" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:97" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="10" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1085,81 +1077,81 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="2:97" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="35"/>
+    <row r="2" spans="1:97" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="22"/>
       <c r="BJ2" s="5"/>
       <c r="BK2" s="11"/>
       <c r="BL2" s="1"/>
       <c r="BM2" s="12"/>
-      <c r="BN2" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="BO2" s="31"/>
-      <c r="BP2" s="31"/>
-      <c r="BQ2" s="31"/>
-      <c r="BR2" s="30"/>
+      <c r="BN2" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="BO2" s="34"/>
+      <c r="BP2" s="34"/>
+      <c r="BQ2" s="34"/>
+      <c r="BR2" s="35"/>
       <c r="BS2" s="13"/>
-      <c r="BT2" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="BU2" s="31"/>
-      <c r="BV2" s="31"/>
-      <c r="BW2" s="30"/>
+      <c r="BT2" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU2" s="34"/>
+      <c r="BV2" s="34"/>
+      <c r="BW2" s="35"/>
       <c r="BX2" s="14"/>
-      <c r="BY2" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="BZ2" s="23"/>
-      <c r="CA2" s="23"/>
-      <c r="CB2" s="32"/>
+      <c r="BY2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="BZ2" s="25"/>
+      <c r="CA2" s="25"/>
+      <c r="CB2" s="36"/>
       <c r="CC2" s="15"/>
-      <c r="CD2" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="CE2" s="23"/>
-      <c r="CF2" s="23"/>
-      <c r="CG2" s="23"/>
-      <c r="CH2" s="23"/>
-      <c r="CI2" s="23"/>
-      <c r="CJ2" s="32"/>
+      <c r="CD2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="CE2" s="25"/>
+      <c r="CF2" s="25"/>
+      <c r="CG2" s="25"/>
+      <c r="CH2" s="25"/>
+      <c r="CI2" s="25"/>
+      <c r="CJ2" s="36"/>
       <c r="CK2" s="16"/>
-      <c r="CL2" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="CM2" s="23"/>
-      <c r="CN2" s="23"/>
-      <c r="CO2" s="23"/>
-      <c r="CP2" s="23"/>
-      <c r="CQ2" s="23"/>
-      <c r="CR2" s="23"/>
-      <c r="CS2" s="23"/>
-    </row>
-    <row r="3" spans="2:97" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="CL2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="CM2" s="25"/>
+      <c r="CN2" s="25"/>
+      <c r="CO2" s="25"/>
+      <c r="CP2" s="25"/>
+      <c r="CQ2" s="25"/>
+      <c r="CR2" s="25"/>
+      <c r="CS2" s="25"/>
+    </row>
+    <row r="3" spans="1:97" s="8" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="27" t="s">
+      <c r="C3" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>27</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
@@ -1181,13 +1173,13 @@
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="2:97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="34"/>
+    <row r="4" spans="1:97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="28"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1308,9 +1300,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:97" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:97" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C5" s="18">
         <v>1</v>
@@ -1328,9 +1320,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:97" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:97" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C6" s="18">
         <v>3</v>
@@ -1348,9 +1340,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:97" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:97" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="20" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C7" s="18">
         <v>7</v>
@@ -1368,9 +1360,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:97" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
-        <v>36</v>
+    <row r="8" spans="1:97" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="18">
         <v>13</v>
@@ -1388,9 +1380,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:97" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="36" t="s">
-        <v>37</v>
+    <row r="9" spans="1:97" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="18">
         <v>14</v>
@@ -1408,78 +1400,99 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:97" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="18">
+    <row r="10" spans="1:97" s="37" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="18">
-        <v>15</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="38"/>
+      <c r="AJ10" s="38"/>
+      <c r="AK10" s="38"/>
+    </row>
+    <row r="11" spans="1:97" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="18">
         <v>16</v>
       </c>
-      <c r="F10" s="18">
-        <v>15</v>
-      </c>
-      <c r="G10" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:97" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="18">
-        <v>8</v>
-      </c>
       <c r="D11" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" s="18">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F11" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:97" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:97" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="20" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C12" s="18">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D12" s="18">
+        <v>1</v>
+      </c>
+      <c r="E12" s="18">
+        <v>17</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1</v>
+      </c>
+      <c r="G12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:97" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="18">
+        <v>18</v>
+      </c>
+      <c r="D13" s="18">
         <v>2</v>
       </c>
-      <c r="E12" s="18">
-        <v>11</v>
-      </c>
-      <c r="F12" s="18">
-        <v>2</v>
-      </c>
-      <c r="G12" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:97" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="18">
-        <v>1</v>
-      </c>
-      <c r="D13" s="18">
-        <v>3</v>
-      </c>
       <c r="E13" s="18">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F13" s="18">
         <v>3</v>
@@ -1488,344 +1501,104 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:97" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:97" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="20" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C14" s="18">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D14" s="18">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18">
+        <v>21</v>
+      </c>
+      <c r="F14" s="18">
+        <v>1</v>
+      </c>
+      <c r="G14" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:97" ht="69" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="21">
+        <v>22</v>
+      </c>
+      <c r="D15" s="18">
         <v>2</v>
       </c>
-      <c r="E14" s="18">
-        <v>11</v>
-      </c>
-      <c r="F14" s="18">
-        <v>2</v>
-      </c>
-      <c r="G14" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:97" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="21">
-        <v>6</v>
-      </c>
-      <c r="D15" s="18">
-        <v>1</v>
-      </c>
       <c r="E15" s="18">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F15" s="18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G15" s="19">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:97" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:97" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C16" s="18">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D16" s="18">
         <v>3</v>
       </c>
       <c r="E16" s="18">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F16" s="18">
         <v>3</v>
       </c>
       <c r="G16" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="18">
+        <v>27</v>
+      </c>
+      <c r="D17" s="18">
         <v>3</v>
       </c>
-      <c r="C17" s="18">
-        <v>9</v>
-      </c>
-      <c r="D17" s="18">
-        <v>6</v>
-      </c>
       <c r="E17" s="18">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F17" s="18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G17" s="19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C18" s="18">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D18" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" s="18">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F18" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="18">
-        <v>9</v>
-      </c>
-      <c r="D19" s="18">
-        <v>4</v>
-      </c>
-      <c r="E19" s="18">
-        <v>8</v>
-      </c>
-      <c r="F19" s="18">
-        <v>5</v>
-      </c>
-      <c r="G19" s="19">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="18">
-        <v>10</v>
-      </c>
-      <c r="D20" s="18">
-        <v>5</v>
-      </c>
-      <c r="E20" s="18">
-        <v>10</v>
-      </c>
-      <c r="F20" s="18">
-        <v>3</v>
-      </c>
-      <c r="G20" s="19">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="18">
-        <v>11</v>
-      </c>
-      <c r="D21" s="18">
-        <v>2</v>
-      </c>
-      <c r="E21" s="18">
-        <v>11</v>
-      </c>
-      <c r="F21" s="18">
-        <v>5</v>
-      </c>
-      <c r="G21" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="18">
-        <v>12</v>
-      </c>
-      <c r="D22" s="18">
-        <v>6</v>
-      </c>
-      <c r="E22" s="18">
-        <v>12</v>
-      </c>
-      <c r="F22" s="18">
-        <v>7</v>
-      </c>
-      <c r="G22" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="18">
-        <v>12</v>
-      </c>
-      <c r="D23" s="18">
-        <v>1</v>
-      </c>
-      <c r="E23" s="18">
-        <v>12</v>
-      </c>
-      <c r="F23" s="18">
-        <v>5</v>
-      </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="18">
-        <v>14</v>
-      </c>
-      <c r="D24" s="18">
-        <v>5</v>
-      </c>
-      <c r="E24" s="18">
-        <v>14</v>
-      </c>
-      <c r="F24" s="18">
-        <v>6</v>
-      </c>
-      <c r="G24" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="18">
-        <v>14</v>
-      </c>
-      <c r="D25" s="18">
-        <v>8</v>
-      </c>
-      <c r="E25" s="18">
-        <v>14</v>
-      </c>
-      <c r="F25" s="18">
-        <v>2</v>
-      </c>
-      <c r="G25" s="19">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="18">
-        <v>14</v>
-      </c>
-      <c r="D26" s="18">
-        <v>7</v>
-      </c>
-      <c r="E26" s="18">
-        <v>14</v>
-      </c>
-      <c r="F26" s="18">
-        <v>3</v>
-      </c>
-      <c r="G26" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="18">
-        <v>15</v>
-      </c>
-      <c r="D27" s="18">
-        <v>4</v>
-      </c>
-      <c r="E27" s="18">
-        <v>15</v>
-      </c>
-      <c r="F27" s="18">
-        <v>8</v>
-      </c>
-      <c r="G27" s="19">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="18">
-        <v>15</v>
-      </c>
-      <c r="D28" s="18">
-        <v>5</v>
-      </c>
-      <c r="E28" s="18">
-        <v>15</v>
-      </c>
-      <c r="F28" s="18">
-        <v>3</v>
-      </c>
-      <c r="G28" s="19">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="18">
-        <v>15</v>
-      </c>
-      <c r="D29" s="18">
-        <v>8</v>
-      </c>
-      <c r="E29" s="18">
-        <v>15</v>
-      </c>
-      <c r="F29" s="18">
-        <v>5</v>
-      </c>
-      <c r="G29" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="18">
-        <v>16</v>
-      </c>
-      <c r="D30" s="18">
-        <v>28</v>
-      </c>
-      <c r="E30" s="18">
-        <v>16</v>
-      </c>
-      <c r="F30" s="18">
-        <v>30</v>
-      </c>
-      <c r="G30" s="19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1843,7 +1616,7 @@
     <mergeCell ref="BY2:CB2"/>
     <mergeCell ref="CD2:CJ2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B31:AK31">
+  <conditionalFormatting sqref="B19:G19">
     <cfRule type="expression" dxfId="9" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -1853,7 +1626,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:AK30">
+  <conditionalFormatting sqref="H5:AK9 H11:AK18">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1880,24 +1653,24 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="BK2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="BK2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="BM2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="BS2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="BX2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="CC2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="CK2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="BM2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="BS2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="BX2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="CC2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="CK2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>